<commit_message>
SSDM-8226 Added search by user email in SampleSearchManagerDBTest.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C75F82C-741E-FF4B-891D-C3C4EFD8DA37}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C70B7E-9743-1E46-B177-2E721CC83BA5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="460" windowWidth="36860" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
+    <workbookView xWindow="1600" yWindow="460" windowWidth="36860" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="162">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -1770,8 +1770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659BE2D9-7405-F646-AD2E-50E30EAAC445}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G86" sqref="G86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1965,38 +1965,50 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="b">
-        <v>0</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C11" t="s">
-        <v>130</v>
-      </c>
-      <c r="D11" t="s">
+    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C12" t="s">
-        <v>130</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="F11" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -3306,63 +3318,72 @@
         <v>159</v>
       </c>
     </row>
-    <row r="83" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B83" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C83" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D83" s="12" t="s">
+    <row r="83" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C83" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E83" s="12" t="s">
+      <c r="E83" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F83" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B84" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C84" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D84" s="12" t="s">
+      <c r="F83" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C84" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E84" s="12" t="s">
+      <c r="E84" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F84" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B85" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C85" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D85" s="12" t="s">
+      <c r="F84" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E85" s="12" t="s">
+      <c r="E85" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F85" s="12" t="s">
+      <c r="F85" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G85" s="1" t="s">
         <v>159</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SSDM-8226 Added another sample which is not related to anything.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C70B7E-9743-1E46-B177-2E721CC83BA5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012C419A-AECA-164C-B2E7-3C1E41E1258D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="460" windowWidth="36860" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
+    <workbookView xWindow="1620" yWindow="460" windowWidth="36800" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="162">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -1770,8 +1770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659BE2D9-7405-F646-AD2E-50E30EAAC445}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G86" sqref="G86"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2079,21 +2079,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C17" s="8" t="s">
+    <row r="17" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="15" t="s">
         <v>87</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -2113,21 +2119,27 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C19" s="8" t="s">
+    <row r="19" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="15" t="s">
         <v>81</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
SSDM-8226 Added experiment type search.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012C419A-AECA-164C-B2E7-3C1E41E1258D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35801E3C-2E68-B141-9925-664C44169039}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="460" windowWidth="36800" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
+    <workbookView xWindow="1600" yWindow="460" windowWidth="36800" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="162">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -1771,7 +1771,7 @@
   <dimension ref="A1:G125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1823,21 +1823,27 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="b">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>89</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1891,21 +1897,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="b">
-        <v>0</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D7" t="s">
+    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>90</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
SSDM-8226 Added search by space in project in experiment. Test code cleanup.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35801E3C-2E68-B141-9925-664C44169039}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527E5164-55B8-324F-8FDF-D601FB74B445}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1600" yWindow="460" windowWidth="36800" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="162">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -1771,7 +1771,7 @@
   <dimension ref="A1:G125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2347,21 +2347,27 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" t="b">
-        <v>0</v>
-      </c>
-      <c r="B31" t="s">
-        <v>137</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D31" t="s">
-        <v>130</v>
-      </c>
-      <c r="E31" t="s">
+    <row r="31" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>49</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -4106,6 +4112,9 @@
         <v>56</v>
       </c>
       <c r="F122" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G122" s="1" t="s">
         <v>159</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SSDM-8226 Created first test for DataSetSearchManager.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527E5164-55B8-324F-8FDF-D601FB74B445}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6366DA56-23A3-BA49-943D-4AB3E1B8B707}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="460" windowWidth="36800" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
+    <workbookView xWindow="1340" yWindow="460" windowWidth="27460" windowHeight="17540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1770,8 +1770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659BE2D9-7405-F646-AD2E-50E30EAAC445}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="C40" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2682,43 +2682,43 @@
         <v>159</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D50" s="1" t="s">
+    <row r="50" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D50" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D51" s="1" t="s">
+      <c r="F50" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D51" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F51" s="12" t="s">
         <v>159</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SSDM-8226 Added new tests for DataSetSearchManager.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6366DA56-23A3-BA49-943D-4AB3E1B8B707}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A761490-8865-4044-A629-F9452512FE35}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="460" windowWidth="27460" windowHeight="17540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
+    <workbookView xWindow="1600" yWindow="460" windowWidth="36800" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="162">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -1770,8 +1770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659BE2D9-7405-F646-AD2E-50E30EAAC445}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C40" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1880,21 +1880,27 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="b">
-        <v>0</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C6" t="s">
-        <v>130</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2023,21 +2029,27 @@
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C13" s="8" t="s">
+    <row r="13" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="15" t="s">
         <v>16</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -2057,38 +2069,50 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C15" s="8" t="s">
+    <row r="15" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="15" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C16" s="8" t="s">
+      <c r="F15" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="15" t="s">
         <v>19</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
SSDM-8226 Made several criteria abstract because they claim to be. Updated criteria.xlsx with criteria for whom the search should be implemented.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A761490-8865-4044-A629-F9452512FE35}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91B7910-34EA-3A4D-96A1-EC779DD6441A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1600" yWindow="460" windowWidth="36800" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="164">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -512,6 +512,12 @@
   </si>
   <si>
     <t>Untested</t>
+  </si>
+  <si>
+    <t>TO-DO</t>
+  </si>
+  <si>
+    <t>No Lucene</t>
   </si>
 </sst>
 </file>
@@ -591,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -613,6 +619,9 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1768,10 +1777,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659BE2D9-7405-F646-AD2E-50E30EAAC445}">
-  <dimension ref="A1:G125"/>
+  <dimension ref="A1:I125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H122" sqref="H122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1781,9 +1790,10 @@
     <col min="3" max="4" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="92.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>154</v>
       </c>
@@ -1805,10 +1815,16 @@
       <c r="G1" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>143</v>
@@ -1823,7 +1839,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="b">
         <v>0</v>
       </c>
@@ -1845,8 +1861,9 @@
       <c r="G3" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="17"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="b">
         <v>0</v>
       </c>
@@ -1862,8 +1879,11 @@
       <c r="E4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="b">
         <v>1</v>
       </c>
@@ -1880,7 +1900,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="b">
         <v>0</v>
       </c>
@@ -1902,8 +1922,9 @@
       <c r="G6" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H6" s="17"/>
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="b">
         <v>0</v>
       </c>
@@ -1925,8 +1946,9 @@
       <c r="G7" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="17"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="b">
         <v>0</v>
       </c>
@@ -1942,8 +1964,11 @@
       <c r="E8" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H8" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="b">
         <v>0</v>
       </c>
@@ -1965,8 +1990,9 @@
       <c r="G9" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="17"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="b">
         <v>0</v>
       </c>
@@ -1982,8 +2008,11 @@
       <c r="E10" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H10" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="b">
         <v>0</v>
       </c>
@@ -2005,8 +2034,9 @@
       <c r="G11" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H11" s="17"/>
+    </row>
+    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="b">
         <v>0</v>
       </c>
@@ -2028,8 +2058,9 @@
       <c r="G12" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H12" s="17"/>
+    </row>
+    <row r="13" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="b">
         <v>0</v>
       </c>
@@ -2051,8 +2082,9 @@
       <c r="G13" s="15" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H13" s="17"/>
+    </row>
+    <row r="14" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="b">
         <v>0</v>
       </c>
@@ -2068,8 +2100,11 @@
       <c r="E14" s="8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H14" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="b">
         <v>0</v>
       </c>
@@ -2091,8 +2126,9 @@
       <c r="G15" s="15" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H15" s="17"/>
+    </row>
+    <row r="16" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="b">
         <v>0</v>
       </c>
@@ -2114,8 +2150,9 @@
       <c r="G16" s="15" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H16" s="17"/>
+    </row>
+    <row r="17" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="b">
         <v>0</v>
       </c>
@@ -2137,8 +2174,9 @@
       <c r="G17" s="15" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H17" s="17"/>
+    </row>
+    <row r="18" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="b">
         <v>0</v>
       </c>
@@ -2154,8 +2192,11 @@
       <c r="E18" s="8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H18" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="b">
         <v>0</v>
       </c>
@@ -2177,8 +2218,9 @@
       <c r="G19" s="15" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H19" s="17"/>
+    </row>
+    <row r="20" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="b">
         <v>0</v>
       </c>
@@ -2200,8 +2242,9 @@
       <c r="G20" s="15" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20" s="17"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="b">
         <v>0</v>
       </c>
@@ -2217,8 +2260,11 @@
       <c r="E21" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H21" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="b">
         <v>1</v>
       </c>
@@ -2235,7 +2281,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="b">
         <v>0</v>
       </c>
@@ -2251,8 +2297,11 @@
       <c r="E23" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H23" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="b">
         <v>0</v>
       </c>
@@ -2268,8 +2317,11 @@
       <c r="E24" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H24" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="b">
         <v>0</v>
       </c>
@@ -2285,8 +2337,11 @@
       <c r="E25" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H25" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="b">
         <v>0</v>
       </c>
@@ -2302,8 +2357,11 @@
       <c r="E26" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H26" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="b">
         <v>1</v>
       </c>
@@ -2320,7 +2378,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="b">
         <v>0</v>
       </c>
@@ -2336,8 +2394,11 @@
       <c r="E28" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H28" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="b">
         <v>0</v>
       </c>
@@ -2353,8 +2414,11 @@
       <c r="E29" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H29" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="b">
         <v>0</v>
       </c>
@@ -2370,8 +2434,11 @@
       <c r="E30" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H30" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="b">
         <v>0</v>
       </c>
@@ -2393,8 +2460,9 @@
       <c r="G31" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H31" s="17"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="b">
         <v>0</v>
       </c>
@@ -2410,8 +2478,11 @@
       <c r="E32" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H32" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="b">
         <v>0</v>
       </c>
@@ -2427,8 +2498,11 @@
       <c r="E33" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H33" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="b">
         <v>0</v>
       </c>
@@ -2444,8 +2518,11 @@
       <c r="E34" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H34" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="b">
         <v>0</v>
       </c>
@@ -2461,8 +2538,11 @@
       <c r="E35" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H35" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="b">
         <v>0</v>
       </c>
@@ -2478,8 +2558,11 @@
       <c r="E36" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H36" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="b">
         <v>0</v>
       </c>
@@ -2495,8 +2578,11 @@
       <c r="E37" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H37" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="b">
         <v>0</v>
       </c>
@@ -2512,8 +2598,11 @@
       <c r="E38" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I38" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="b">
         <v>0</v>
       </c>
@@ -2529,8 +2618,11 @@
       <c r="E39" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H39" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="b">
         <v>0</v>
       </c>
@@ -2546,8 +2638,11 @@
       <c r="E40" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H40" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="b">
         <v>0</v>
       </c>
@@ -2563,8 +2658,11 @@
       <c r="E41" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H41" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="b">
         <v>0</v>
       </c>
@@ -2580,8 +2678,11 @@
       <c r="E42" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H42" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="b">
         <v>0</v>
       </c>
@@ -2597,8 +2698,11 @@
       <c r="E43" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H43" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="b">
         <v>0</v>
       </c>
@@ -2614,8 +2718,11 @@
       <c r="E44" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H44" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="b">
         <v>0</v>
       </c>
@@ -2631,8 +2738,11 @@
       <c r="E45" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H45" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="b">
         <v>0</v>
       </c>
@@ -2648,8 +2758,11 @@
       <c r="E46" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H46" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="b">
         <v>0</v>
       </c>
@@ -2665,8 +2778,11 @@
       <c r="E47" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H47" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="b">
         <v>0</v>
       </c>
@@ -2682,8 +2798,11 @@
       <c r="E48" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H48" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="b">
         <v>0</v>
       </c>
@@ -2705,8 +2824,9 @@
       <c r="G49" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H49" s="17"/>
+    </row>
+    <row r="50" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="12" t="b">
         <v>0</v>
       </c>
@@ -2725,8 +2845,11 @@
       <c r="F50" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H50" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="12" t="b">
         <v>0</v>
       </c>
@@ -2745,8 +2868,11 @@
       <c r="F51" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H51" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="b">
         <v>0</v>
       </c>
@@ -2768,8 +2894,9 @@
       <c r="G52" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H52" s="17"/>
+    </row>
+    <row r="53" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="b">
         <v>0</v>
       </c>
@@ -2791,8 +2918,9 @@
       <c r="G53" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H53" s="17"/>
+    </row>
+    <row r="54" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="b">
         <v>0</v>
       </c>
@@ -2814,8 +2942,9 @@
       <c r="G54" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H54" s="17"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="b">
         <v>0</v>
       </c>
@@ -2831,8 +2960,11 @@
       <c r="E55" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H55" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="b">
         <v>0</v>
       </c>
@@ -2848,8 +2980,11 @@
       <c r="E56" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H56" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="b">
         <v>0</v>
       </c>
@@ -2865,8 +3000,11 @@
       <c r="E57" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H57" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="b">
         <v>0</v>
       </c>
@@ -2882,8 +3020,11 @@
       <c r="E58" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H58" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="b">
         <v>0</v>
       </c>
@@ -2899,8 +3040,11 @@
       <c r="E59" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H59" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="b">
         <v>0</v>
       </c>
@@ -2916,8 +3060,11 @@
       <c r="E60" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H60" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="b">
         <v>0</v>
       </c>
@@ -2933,8 +3080,11 @@
       <c r="E61" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H61" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="b">
         <v>0</v>
       </c>
@@ -2956,8 +3106,9 @@
       <c r="G62" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H62" s="17"/>
+    </row>
+    <row r="63" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="12" t="b">
         <v>0</v>
       </c>
@@ -2976,8 +3127,11 @@
       <c r="F63" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H63" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="12" t="b">
         <v>0</v>
       </c>
@@ -2996,8 +3150,11 @@
       <c r="F64" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H64" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="12" t="b">
         <v>0</v>
       </c>
@@ -3016,8 +3173,11 @@
       <c r="F65" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H65" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="b">
         <v>0</v>
       </c>
@@ -3039,8 +3199,9 @@
       <c r="G66" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H66" s="17"/>
+    </row>
+    <row r="67" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="b">
         <v>0</v>
       </c>
@@ -3062,8 +3223,9 @@
       <c r="G67" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H67" s="17"/>
+    </row>
+    <row r="68" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="b">
         <v>0</v>
       </c>
@@ -3085,8 +3247,9 @@
       <c r="G68" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H68" s="17"/>
+    </row>
+    <row r="69" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="12" t="b">
         <v>0</v>
       </c>
@@ -3105,8 +3268,11 @@
       <c r="F69" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H69" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="12" t="b">
         <v>0</v>
       </c>
@@ -3125,8 +3291,11 @@
       <c r="F70" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H70" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="12" t="b">
         <v>0</v>
       </c>
@@ -3145,8 +3314,11 @@
       <c r="F71" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H71" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="b">
         <v>0</v>
       </c>
@@ -3168,8 +3340,9 @@
       <c r="G72" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H72" s="17"/>
+    </row>
+    <row r="73" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="b">
         <v>0</v>
       </c>
@@ -3191,8 +3364,9 @@
       <c r="G73" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H73" s="17"/>
+    </row>
+    <row r="74" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="12" t="b">
         <v>0</v>
       </c>
@@ -3211,8 +3385,11 @@
       <c r="F74" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H74" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="12" t="b">
         <v>0</v>
       </c>
@@ -3231,8 +3408,11 @@
       <c r="F75" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H75" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="12" t="b">
         <v>0</v>
       </c>
@@ -3251,8 +3431,11 @@
       <c r="F76" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H76" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="12" t="b">
         <v>0</v>
       </c>
@@ -3271,8 +3454,11 @@
       <c r="F77" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H77" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="12" t="b">
         <v>0</v>
       </c>
@@ -3291,8 +3477,11 @@
       <c r="F78" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H78" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="12" t="b">
         <v>0</v>
       </c>
@@ -3311,8 +3500,11 @@
       <c r="F79" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H79" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="12" t="b">
         <v>0</v>
       </c>
@@ -3331,8 +3523,11 @@
       <c r="F80" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H80" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="12" t="b">
         <v>0</v>
       </c>
@@ -3351,8 +3546,11 @@
       <c r="F81" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H81" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="12" t="b">
         <v>0</v>
       </c>
@@ -3371,8 +3569,11 @@
       <c r="F82" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H82" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="b">
         <v>0</v>
       </c>
@@ -3394,8 +3595,9 @@
       <c r="G83" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H83" s="17"/>
+    </row>
+    <row r="84" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="b">
         <v>0</v>
       </c>
@@ -3417,8 +3619,9 @@
       <c r="G84" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H84" s="17"/>
+    </row>
+    <row r="85" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="b">
         <v>0</v>
       </c>
@@ -3440,8 +3643,9 @@
       <c r="G85" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H85" s="17"/>
+    </row>
+    <row r="86" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="12" t="b">
         <v>0</v>
       </c>
@@ -3460,8 +3664,11 @@
       <c r="F86" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H86" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="12" t="b">
         <v>0</v>
       </c>
@@ -3480,8 +3687,11 @@
       <c r="F87" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H87" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="12" t="b">
         <v>0</v>
       </c>
@@ -3500,8 +3710,11 @@
       <c r="F88" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H88" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="12" t="b">
         <v>0</v>
       </c>
@@ -3520,8 +3733,11 @@
       <c r="F89" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H89" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="12" t="b">
         <v>0</v>
       </c>
@@ -3540,8 +3756,11 @@
       <c r="F90" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H90" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="12" t="b">
         <v>0</v>
       </c>
@@ -3560,8 +3779,11 @@
       <c r="F91" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H91" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="12" t="b">
         <v>0</v>
       </c>
@@ -3580,8 +3802,11 @@
       <c r="F92" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H92" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="12" t="b">
         <v>0</v>
       </c>
@@ -3600,8 +3825,11 @@
       <c r="F93" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H93" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="b">
         <v>1</v>
       </c>
@@ -3618,7 +3846,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="b">
         <v>1</v>
       </c>
@@ -3635,7 +3863,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="96" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="b">
         <v>0</v>
       </c>
@@ -3657,8 +3885,9 @@
       <c r="G96" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H96" s="17"/>
+    </row>
+    <row r="97" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="b">
         <v>0</v>
       </c>
@@ -3680,8 +3909,9 @@
       <c r="G97" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H97" s="17"/>
+    </row>
+    <row r="98" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="b">
         <v>0</v>
       </c>
@@ -3703,8 +3933,9 @@
       <c r="G98" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H98" s="17"/>
+    </row>
+    <row r="99" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="b">
         <v>0</v>
       </c>
@@ -3726,8 +3957,9 @@
       <c r="G99" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H99" s="17"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="9" t="b">
         <v>1</v>
       </c>
@@ -3744,7 +3976,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="9" t="b">
         <v>1</v>
       </c>
@@ -3761,7 +3993,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="102" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="14" t="b">
         <v>0</v>
       </c>
@@ -3783,8 +4015,9 @@
       <c r="G102" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H102" s="17"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="9" t="b">
         <v>0</v>
       </c>
@@ -3800,8 +4033,11 @@
       <c r="E103" s="9" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H103" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="9" t="b">
         <v>0</v>
       </c>
@@ -3817,8 +4053,11 @@
       <c r="E104" s="9" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H104" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="9" t="b">
         <v>0</v>
       </c>
@@ -3834,8 +4073,11 @@
       <c r="E105" s="9" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H105" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="9" t="b">
         <v>0</v>
       </c>
@@ -3851,8 +4093,11 @@
       <c r="E106" s="9" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H106" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="9" t="b">
         <v>0</v>
       </c>
@@ -3868,8 +4113,11 @@
       <c r="E107" s="9" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H107" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="9" t="b">
         <v>0</v>
       </c>
@@ -3885,10 +4133,13 @@
       <c r="E108" s="9" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H108" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B109" t="s">
         <v>150</v>
@@ -3903,7 +4154,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="b">
         <v>0</v>
       </c>
@@ -3919,8 +4170,11 @@
       <c r="E110" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H110" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="b">
         <v>0</v>
       </c>
@@ -3936,8 +4190,11 @@
       <c r="E111" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H111" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="b">
         <v>0</v>
       </c>
@@ -3953,8 +4210,11 @@
       <c r="E112" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H112" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="b">
         <v>0</v>
       </c>
@@ -3970,8 +4230,11 @@
       <c r="E113" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H113" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="b">
         <v>0</v>
       </c>
@@ -3987,8 +4250,11 @@
       <c r="E114" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H114" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="b">
         <v>0</v>
       </c>
@@ -4004,8 +4270,11 @@
       <c r="E115" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H115" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="b">
         <v>0</v>
       </c>
@@ -4021,8 +4290,11 @@
       <c r="E116" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H116" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="b">
         <v>0</v>
       </c>
@@ -4038,8 +4310,11 @@
       <c r="E117" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H117" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="b">
         <v>1</v>
       </c>
@@ -4056,7 +4331,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="119" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="b">
         <v>1</v>
       </c>
@@ -4078,8 +4353,9 @@
       <c r="G119" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H119" s="17"/>
+    </row>
+    <row r="120" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="b">
         <v>1</v>
       </c>
@@ -4101,8 +4377,9 @@
       <c r="G120" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H120" s="17"/>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="b">
         <v>1</v>
       </c>
@@ -4119,7 +4396,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="122" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="b">
         <v>1</v>
       </c>
@@ -4141,8 +4418,9 @@
       <c r="G122" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H122" s="17"/>
+    </row>
+    <row r="123" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="b">
         <v>1</v>
       </c>
@@ -4164,8 +4442,9 @@
       <c r="G123" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H123" s="17"/>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="b">
         <v>0</v>
       </c>
@@ -4181,8 +4460,11 @@
       <c r="E124" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H124" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="9" t="b">
         <v>0</v>
       </c>
@@ -4197,6 +4479,9 @@
       </c>
       <c r="E125" s="9" t="s">
         <v>111</v>
+      </c>
+      <c r="H125" s="18" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -4207,5 +4492,6 @@
     <sortCondition ref="E2:E125"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SSDM-8226 Reviewed which other criteria should be checked, whether we should implement search for them.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91B7910-34EA-3A4D-96A1-EC779DD6441A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B851CA7A-7D43-CF4E-93C9-DFB2B989A263}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1600" yWindow="460" windowWidth="36800" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
@@ -1780,7 +1780,7 @@
   <dimension ref="A1:I125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A81" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H122" sqref="H122"/>
+      <selection activeCell="H109" sqref="H109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
SSDM-8226 Made testSearchWithExperimentWithIdSetToIdentifier() test work.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B851CA7A-7D43-CF4E-93C9-DFB2B989A263}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45ACBBE-F67A-174F-9AF3-F41AC6CD4098}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="460" windowWidth="36800" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
+    <workbookView xWindow="1220" yWindow="460" windowWidth="27580" windowHeight="17540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="164">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -1779,8 +1779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659BE2D9-7405-F646-AD2E-50E30EAAC445}">
   <dimension ref="A1:I125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H109" sqref="H109"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2176,25 +2176,29 @@
       </c>
       <c r="H17" s="17"/>
     </row>
-    <row r="18" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="B18" s="8" t="s">
+    <row r="18" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="H18" s="18" t="s">
-        <v>159</v>
-      </c>
+      <c r="F18" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="H18" s="17"/>
     </row>
     <row r="19" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="b">

</xml_diff>

<commit_message>
SSDM-8226 Updated criteria.xlsx with which criteria use Lucene and which ones do not. Commented out the tests in SearchSampleTest, which are no longer relevant to the new search engine.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45ACBBE-F67A-174F-9AF3-F41AC6CD4098}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01002E5-4433-BF46-9D88-CA1421EF374B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="460" windowWidth="27580" windowHeight="17540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
+    <workbookView xWindow="1600" yWindow="460" windowWidth="36800" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="169">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -518,13 +518,28 @@
   </si>
   <si>
     <t>No Lucene</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>we have no caching in the new search engine.</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>get rid of SortOrder, it makes sence only for full text search.</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -536,6 +551,21 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11.3"/>
+      <color rgb="FF0073BF"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -597,7 +627,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -610,7 +640,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -622,6 +651,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1777,10 +1808,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659BE2D9-7405-F646-AD2E-50E30EAAC445}">
-  <dimension ref="A1:I125"/>
+  <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1790,7 +1821,7 @@
     <col min="3" max="4" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="92.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="18"/>
+    <col min="8" max="9" width="10.83203125" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1815,35 +1846,39 @@
       <c r="G1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="16" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="b">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>143</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1861,7 +1896,8 @@
       <c r="G3" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H3" s="17"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="b">
@@ -1879,7 +1915,7 @@
       <c r="E4" t="s">
         <v>118</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="17" t="s">
         <v>159</v>
       </c>
     </row>
@@ -1899,12 +1935,24 @@
       <c r="E5" t="s">
         <v>84</v>
       </c>
+      <c r="F5" t="s">
+        <v>168</v>
+      </c>
+      <c r="G5" t="s">
+        <v>168</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>143</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1922,13 +1970,14 @@
       <c r="G6" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H6" s="17"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>143</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1946,7 +1995,8 @@
       <c r="G7" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H7" s="17"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="b">
@@ -1964,7 +2014,7 @@
       <c r="E8" t="s">
         <v>117</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="17" t="s">
         <v>159</v>
       </c>
     </row>
@@ -1972,7 +2022,7 @@
       <c r="A9" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>143</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1990,7 +2040,8 @@
       <c r="G9" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H9" s="17"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="b">
@@ -2008,7 +2059,7 @@
       <c r="E10" t="s">
         <v>48</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="I10" s="17" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2016,7 +2067,7 @@
       <c r="A11" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>143</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -2034,13 +2085,14 @@
       <c r="G11" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H11" s="17"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
     </row>
     <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>143</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -2058,217 +2110,227 @@
       <c r="G12" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H12" s="17"/>
-    </row>
-    <row r="13" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="B13" s="15" t="s">
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+    </row>
+    <row r="13" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="H13" s="17"/>
-    </row>
-    <row r="14" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="B14" s="8" t="s">
+      <c r="F13" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+    </row>
+    <row r="14" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="B15" s="15" t="s">
+      <c r="H14" s="16"/>
+      <c r="I14" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="H15" s="17"/>
-    </row>
-    <row r="16" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="B16" s="15" t="s">
+      <c r="F15" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+    </row>
+    <row r="16" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="B16" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="H16" s="17"/>
-    </row>
-    <row r="17" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="B17" s="15" t="s">
+      <c r="F16" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+    </row>
+    <row r="17" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="B17" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F17" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="H17" s="17"/>
-    </row>
-    <row r="18" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="B18" s="15" t="s">
+      <c r="F17" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+    </row>
+    <row r="18" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="F18" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="H18" s="17"/>
-    </row>
-    <row r="19" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="B19" s="15" t="s">
+      <c r="F18" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+    </row>
+    <row r="19" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="B19" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="F19" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="H19" s="17"/>
-    </row>
-    <row r="20" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="B20" s="15" t="s">
+      <c r="F19" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+    </row>
+    <row r="20" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="B20" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="F20" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="H20" s="17"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="b">
-        <v>0</v>
-      </c>
-      <c r="B21" t="s">
-        <v>137</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="F20" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+    </row>
+    <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C21" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H21" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H21" s="16"/>
+      <c r="I21" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="b">
         <v>1</v>
       </c>
@@ -2284,8 +2346,20 @@
       <c r="E22" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F22" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="I22" s="17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="b">
         <v>0</v>
       </c>
@@ -2301,71 +2375,77 @@
       <c r="E23" t="s">
         <v>39</v>
       </c>
-      <c r="H23" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" t="b">
-        <v>0</v>
-      </c>
-      <c r="B24" t="s">
-        <v>137</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="H23" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C24" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H24" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="b">
-        <v>0</v>
-      </c>
-      <c r="B25" t="s">
-        <v>137</v>
-      </c>
-      <c r="C25" s="2" t="s">
+      <c r="H24" s="16"/>
+      <c r="I24" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H25" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="b">
-        <v>0</v>
-      </c>
-      <c r="B26" t="s">
-        <v>137</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="H25" s="16"/>
+      <c r="I25" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H26" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H26" s="16"/>
+      <c r="I26" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="b">
         <v>1</v>
       </c>
@@ -2382,7 +2462,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="b">
         <v>0</v>
       </c>
@@ -2398,58 +2478,57 @@
       <c r="E28" t="s">
         <v>3</v>
       </c>
-      <c r="H28" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" t="b">
-        <v>0</v>
-      </c>
-      <c r="B29" t="s">
-        <v>137</v>
-      </c>
-      <c r="C29" s="2" t="s">
+    </row>
+    <row r="29" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C29" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" t="b">
-        <v>0</v>
-      </c>
-      <c r="B30" t="s">
-        <v>137</v>
-      </c>
-      <c r="C30" s="2" t="s">
+      <c r="H29" s="16"/>
+      <c r="I29" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C30" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H30" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H30" s="16"/>
+      <c r="I30" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="15" t="s">
         <v>143</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -2464,285 +2543,316 @@
       <c r="G31" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H31" s="17"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" t="b">
-        <v>0</v>
-      </c>
-      <c r="B32" t="s">
-        <v>137</v>
-      </c>
-      <c r="C32" s="2" t="s">
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+    </row>
+    <row r="32" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C32" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H32" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" t="b">
-        <v>0</v>
-      </c>
-      <c r="B33" t="s">
-        <v>137</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="F32" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+    </row>
+    <row r="33" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C33" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H33" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" t="b">
-        <v>0</v>
-      </c>
-      <c r="B34" t="s">
-        <v>137</v>
-      </c>
-      <c r="C34" s="2" t="s">
+      <c r="H33" s="16"/>
+      <c r="I33" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C34" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H34" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" t="b">
-        <v>0</v>
-      </c>
-      <c r="B35" t="s">
-        <v>137</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="H34" s="16"/>
+      <c r="I34" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C35" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H35" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" t="b">
-        <v>0</v>
-      </c>
-      <c r="B36" t="s">
-        <v>137</v>
-      </c>
-      <c r="C36" s="2" t="s">
+      <c r="H35" s="16"/>
+      <c r="I35" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C36" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="H36" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" t="b">
-        <v>0</v>
-      </c>
-      <c r="B37" t="s">
-        <v>137</v>
-      </c>
-      <c r="C37" s="2" t="s">
+      <c r="F36" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+    </row>
+    <row r="37" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C37" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H37" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" t="b">
-        <v>0</v>
-      </c>
-      <c r="B38" t="s">
-        <v>137</v>
-      </c>
-      <c r="C38" s="2" t="s">
+      <c r="H37" s="16"/>
+      <c r="I37" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C38" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="I38" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" t="b">
-        <v>0</v>
-      </c>
-      <c r="B39" t="s">
-        <v>137</v>
-      </c>
-      <c r="C39" s="2" t="s">
+      <c r="H38" s="16"/>
+      <c r="I38" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C39" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H39" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" t="b">
-        <v>0</v>
-      </c>
-      <c r="B40" t="s">
-        <v>137</v>
-      </c>
-      <c r="C40" s="2" t="s">
+      <c r="H39" s="16"/>
+      <c r="I39" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C40" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="H40" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" t="b">
-        <v>0</v>
-      </c>
-      <c r="B41" t="s">
-        <v>137</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="H40" s="16"/>
+      <c r="I40" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C41" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H41" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" t="b">
-        <v>0</v>
-      </c>
-      <c r="B42" t="s">
-        <v>137</v>
-      </c>
-      <c r="C42" s="2" t="s">
+      <c r="H41" s="16"/>
+      <c r="I41" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C42" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="H42" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" t="b">
-        <v>0</v>
-      </c>
-      <c r="B43" t="s">
-        <v>137</v>
-      </c>
-      <c r="C43" s="2" t="s">
+      <c r="F42" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+    </row>
+    <row r="43" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C43" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H43" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" t="b">
-        <v>0</v>
-      </c>
-      <c r="B44" t="s">
-        <v>137</v>
-      </c>
-      <c r="C44" s="2" t="s">
+      <c r="F43" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+    </row>
+    <row r="44" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C44" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="H44" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" t="b">
-        <v>0</v>
-      </c>
-      <c r="B45" t="s">
-        <v>137</v>
-      </c>
-      <c r="C45" s="2" t="s">
+      <c r="H44" s="16"/>
+      <c r="I44" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C45" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="H45" s="18" t="s">
+      <c r="H45" s="16"/>
+      <c r="I45" s="16" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2762,8 +2872,11 @@
       <c r="E46" t="s">
         <v>25</v>
       </c>
-      <c r="H46" s="18" t="s">
-        <v>159</v>
+      <c r="H46" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I46" s="17" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -2782,8 +2895,11 @@
       <c r="E47" t="s">
         <v>34</v>
       </c>
-      <c r="H47" s="18" t="s">
-        <v>159</v>
+      <c r="H47" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I47" s="17" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -2802,18 +2918,21 @@
       <c r="E48" t="s">
         <v>38</v>
       </c>
-      <c r="H48" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H48" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I48" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C49" s="9" t="s">
         <v>151</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -2828,62 +2947,61 @@
       <c r="G49" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H49" s="17"/>
-    </row>
-    <row r="50" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D50" s="12" t="s">
+      <c r="H49" s="16"/>
+      <c r="I49" s="16"/>
+    </row>
+    <row r="50" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D50" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E50" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="F50" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H50" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D51" s="12" t="s">
+      <c r="F50" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+    </row>
+    <row r="51" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D51" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="E51" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F51" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H51" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F51" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+    </row>
+    <row r="52" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C52" s="9" t="s">
         <v>151</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -2898,16 +3016,17 @@
       <c r="G52" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H52" s="17"/>
-    </row>
-    <row r="53" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H52" s="16"/>
+      <c r="I52" s="16"/>
+    </row>
+    <row r="53" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C53" s="9" t="s">
         <v>151</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -2922,16 +3041,17 @@
       <c r="G53" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H53" s="17"/>
-    </row>
-    <row r="54" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H53" s="16"/>
+      <c r="I53" s="16"/>
+    </row>
+    <row r="54" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C54" s="9" t="s">
         <v>151</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -2946,9 +3066,10 @@
       <c r="G54" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H54" s="17"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H54" s="16"/>
+      <c r="I54" s="16"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="b">
         <v>0</v>
       </c>
@@ -2964,11 +3085,14 @@
       <c r="E55" t="s">
         <v>17</v>
       </c>
-      <c r="H55" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H55" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I55" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="b">
         <v>0</v>
       </c>
@@ -2984,11 +3108,14 @@
       <c r="E56" t="s">
         <v>20</v>
       </c>
-      <c r="H56" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H56" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I56" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="b">
         <v>0</v>
       </c>
@@ -3004,11 +3131,14 @@
       <c r="E57" t="s">
         <v>2</v>
       </c>
-      <c r="H57" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H57" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I57" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="b">
         <v>0</v>
       </c>
@@ -3024,11 +3154,14 @@
       <c r="E58" t="s">
         <v>45</v>
       </c>
-      <c r="H58" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H58" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I58" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="b">
         <v>0</v>
       </c>
@@ -3044,11 +3177,14 @@
       <c r="E59" t="s">
         <v>43</v>
       </c>
-      <c r="H59" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H59" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I59" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="b">
         <v>0</v>
       </c>
@@ -3064,11 +3200,14 @@
       <c r="E60" t="s">
         <v>44</v>
       </c>
-      <c r="H60" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H60" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I60" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="b">
         <v>0</v>
       </c>
@@ -3084,18 +3223,21 @@
       <c r="E61" t="s">
         <v>109</v>
       </c>
-      <c r="H61" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H61" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I61" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="C62" s="9" t="s">
         <v>151</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -3110,85 +3252,83 @@
       <c r="G62" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H62" s="17"/>
-    </row>
-    <row r="63" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B63" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C63" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D63" s="12" t="s">
+      <c r="H62" s="16"/>
+      <c r="I62" s="16"/>
+    </row>
+    <row r="63" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D63" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="E63" s="12" t="s">
+      <c r="E63" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F63" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H63" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B64" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C64" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D64" s="12" t="s">
+      <c r="F63" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H63" s="18"/>
+      <c r="I63" s="18"/>
+    </row>
+    <row r="64" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D64" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="E64" s="12" t="s">
+      <c r="E64" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F64" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H64" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B65" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C65" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D65" s="12" t="s">
+      <c r="F64" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H64" s="18"/>
+      <c r="I64" s="18"/>
+    </row>
+    <row r="65" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D65" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="E65" s="12" t="s">
+      <c r="E65" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F65" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H65" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F65" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H65" s="18"/>
+      <c r="I65" s="18"/>
+    </row>
+    <row r="66" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C66" s="10" t="s">
+      <c r="C66" s="9" t="s">
         <v>151</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -3203,16 +3343,17 @@
       <c r="G66" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H66" s="17"/>
-    </row>
-    <row r="67" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H66" s="16"/>
+      <c r="I66" s="16"/>
+    </row>
+    <row r="67" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C67" s="10" t="s">
+      <c r="C67" s="9" t="s">
         <v>151</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -3227,16 +3368,17 @@
       <c r="G67" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H67" s="17"/>
-    </row>
-    <row r="68" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H67" s="16"/>
+      <c r="I67" s="16"/>
+    </row>
+    <row r="68" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C68" s="10" t="s">
+      <c r="C68" s="9" t="s">
         <v>151</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -3251,85 +3393,86 @@
       <c r="G68" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H68" s="17"/>
-    </row>
-    <row r="69" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B69" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C69" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D69" s="12" t="s">
+      <c r="H68" s="16"/>
+      <c r="I68" s="16"/>
+    </row>
+    <row r="69" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D69" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E69" s="12" t="s">
+      <c r="E69" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="F69" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H69" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B70" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C70" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D70" s="12" t="s">
+      <c r="F69" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H69" s="18"/>
+      <c r="I69" s="18"/>
+    </row>
+    <row r="70" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E70" s="12" t="s">
+      <c r="E70" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F70" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H70" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B71" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C71" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D71" s="12" t="s">
+      <c r="F70" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H70" s="16"/>
+      <c r="I70" s="16"/>
+    </row>
+    <row r="71" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B71" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C71" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D71" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E71" s="12" t="s">
+      <c r="E71" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="F71" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H71" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F71" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H71" s="18"/>
+      <c r="I71" s="18"/>
+    </row>
+    <row r="72" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C72" s="10" t="s">
+      <c r="C72" s="9" t="s">
         <v>151</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -3344,16 +3487,17 @@
       <c r="G72" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H72" s="17"/>
-    </row>
-    <row r="73" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H72" s="16"/>
+      <c r="I72" s="16"/>
+    </row>
+    <row r="73" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C73" s="10" t="s">
+      <c r="C73" s="9" t="s">
         <v>151</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -3368,223 +3512,218 @@
       <c r="G73" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H73" s="17"/>
-    </row>
-    <row r="74" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B74" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C74" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D74" s="12" t="s">
+      <c r="H73" s="16"/>
+      <c r="I73" s="16"/>
+    </row>
+    <row r="74" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B74" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C74" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D74" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E74" s="12" t="s">
+      <c r="E74" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F74" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H74" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B75" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C75" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D75" s="12" t="s">
+      <c r="F74" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H74" s="18"/>
+      <c r="I74" s="18"/>
+    </row>
+    <row r="75" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B75" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C75" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D75" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E75" s="12" t="s">
+      <c r="E75" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F75" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H75" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B76" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C76" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D76" s="12" t="s">
+      <c r="F75" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H75" s="18"/>
+      <c r="I75" s="18"/>
+    </row>
+    <row r="76" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B76" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D76" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E76" s="12" t="s">
+      <c r="E76" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F76" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H76" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B77" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C77" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D77" s="12" t="s">
+      <c r="F76" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H76" s="18"/>
+      <c r="I76" s="18"/>
+    </row>
+    <row r="77" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B77" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C77" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D77" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E77" s="12" t="s">
+      <c r="E77" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F77" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H77" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B78" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C78" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D78" s="12" t="s">
+      <c r="F77" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H77" s="18"/>
+      <c r="I77" s="18"/>
+    </row>
+    <row r="78" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B78" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D78" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E78" s="12" t="s">
+      <c r="E78" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F78" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H78" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B79" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C79" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D79" s="12" t="s">
+      <c r="F78" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H78" s="18"/>
+      <c r="I78" s="18"/>
+    </row>
+    <row r="79" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B79" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C79" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D79" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E79" s="12" t="s">
+      <c r="E79" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F79" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H79" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B80" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C80" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D80" s="12" t="s">
+      <c r="F79" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H79" s="18"/>
+      <c r="I79" s="18"/>
+    </row>
+    <row r="80" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B80" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C80" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D80" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E80" s="12" t="s">
+      <c r="E80" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F80" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H80" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B81" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C81" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D81" s="12" t="s">
+      <c r="F80" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H80" s="18"/>
+      <c r="I80" s="18"/>
+    </row>
+    <row r="81" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B81" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C81" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D81" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E81" s="12" t="s">
+      <c r="E81" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F81" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H81" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B82" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C82" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D82" s="12" t="s">
+      <c r="F81" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H81" s="18"/>
+      <c r="I81" s="18"/>
+    </row>
+    <row r="82" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E82" s="12" t="s">
+      <c r="E82" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F82" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H82" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F82" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H82" s="16"/>
+      <c r="I82" s="16"/>
+    </row>
+    <row r="83" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C83" s="10" t="s">
+      <c r="C83" s="9" t="s">
         <v>151</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -3599,16 +3738,17 @@
       <c r="G83" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H83" s="17"/>
-    </row>
-    <row r="84" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H83" s="16"/>
+      <c r="I83" s="16"/>
+    </row>
+    <row r="84" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C84" s="10" t="s">
+      <c r="C84" s="9" t="s">
         <v>151</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -3623,16 +3763,17 @@
       <c r="G84" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H84" s="17"/>
-    </row>
-    <row r="85" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H84" s="16"/>
+      <c r="I84" s="16"/>
+    </row>
+    <row r="85" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C85" s="10" t="s">
+      <c r="C85" s="9" t="s">
         <v>151</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -3647,193 +3788,186 @@
       <c r="G85" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H85" s="17"/>
-    </row>
-    <row r="86" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B86" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C86" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D86" s="12" t="s">
+      <c r="H85" s="16"/>
+      <c r="I85" s="16"/>
+    </row>
+    <row r="86" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B86" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C86" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D86" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E86" s="12" t="s">
+      <c r="E86" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="F86" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H86" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B87" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C87" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D87" s="12" t="s">
+      <c r="F86" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H86" s="18"/>
+      <c r="I86" s="18"/>
+    </row>
+    <row r="87" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B87" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C87" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D87" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E87" s="12" t="s">
+      <c r="E87" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="F87" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H87" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B88" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C88" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D88" s="12" t="s">
+      <c r="F87" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H87" s="18"/>
+      <c r="I87" s="18"/>
+    </row>
+    <row r="88" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B88" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C88" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D88" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E88" s="12" t="s">
+      <c r="E88" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="F88" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H88" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B89" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C89" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D89" s="12" t="s">
+      <c r="F88" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H88" s="18"/>
+      <c r="I88" s="18"/>
+    </row>
+    <row r="89" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B89" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C89" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D89" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E89" s="12" t="s">
+      <c r="E89" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="F89" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H89" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B90" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C90" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D90" s="12" t="s">
+      <c r="F89" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H89" s="18"/>
+      <c r="I89" s="18"/>
+    </row>
+    <row r="90" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B90" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C90" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D90" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E90" s="12" t="s">
+      <c r="E90" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="F90" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H90" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B91" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C91" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D91" s="12" t="s">
+      <c r="F90" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H90" s="18"/>
+      <c r="I90" s="18"/>
+    </row>
+    <row r="91" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B91" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C91" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D91" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E91" s="12" t="s">
+      <c r="E91" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="F91" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H91" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B92" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C92" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D92" s="12" t="s">
+      <c r="F91" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H91" s="18"/>
+      <c r="I91" s="18"/>
+    </row>
+    <row r="92" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B92" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C92" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D92" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E92" s="12" t="s">
+      <c r="E92" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="F92" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H92" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B93" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C93" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D93" s="12" t="s">
+      <c r="F92" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H92" s="18"/>
+      <c r="I92" s="18"/>
+    </row>
+    <row r="93" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B93" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C93" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D93" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E93" s="12" t="s">
+      <c r="E93" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="F93" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H93" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F93" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H93" s="18"/>
+      <c r="I93" s="18"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="b">
         <v>1</v>
       </c>
@@ -3849,8 +3983,20 @@
       <c r="E94" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F94" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="G94" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="H94" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="I94" s="18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="b">
         <v>1</v>
       </c>
@@ -3866,8 +4012,20 @@
       <c r="E95" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F95" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="G95" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="H95" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="I95" s="18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="b">
         <v>0</v>
       </c>
@@ -3877,7 +4035,7 @@
       <c r="C96" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D96" s="11" t="s">
+      <c r="D96" s="10" t="s">
         <v>150</v>
       </c>
       <c r="E96" s="1" t="s">
@@ -3889,9 +4047,10 @@
       <c r="G96" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H96" s="17"/>
-    </row>
-    <row r="97" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H96" s="16"/>
+      <c r="I96" s="16"/>
+    </row>
+    <row r="97" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="b">
         <v>0</v>
       </c>
@@ -3901,7 +4060,7 @@
       <c r="C97" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D97" s="11" t="s">
+      <c r="D97" s="10" t="s">
         <v>150</v>
       </c>
       <c r="E97" s="1" t="s">
@@ -3913,9 +4072,10 @@
       <c r="G97" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H97" s="17"/>
-    </row>
-    <row r="98" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H97" s="16"/>
+      <c r="I97" s="16"/>
+    </row>
+    <row r="98" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="b">
         <v>0</v>
       </c>
@@ -3925,7 +4085,7 @@
       <c r="C98" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D98" s="11" t="s">
+      <c r="D98" s="10" t="s">
         <v>150</v>
       </c>
       <c r="E98" s="1" t="s">
@@ -3937,9 +4097,10 @@
       <c r="G98" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H98" s="17"/>
-    </row>
-    <row r="99" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H98" s="16"/>
+      <c r="I98" s="16"/>
+    </row>
+    <row r="99" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="b">
         <v>0</v>
       </c>
@@ -3949,7 +4110,7 @@
       <c r="C99" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D99" s="11" t="s">
+      <c r="D99" s="10" t="s">
         <v>150</v>
       </c>
       <c r="E99" s="1" t="s">
@@ -3961,56 +4122,81 @@
       <c r="G99" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H99" s="17"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" s="9" t="b">
+      <c r="H99" s="16"/>
+      <c r="I99" s="16"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A100" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="B100" s="9" t="s">
+      <c r="B100" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="C100" s="9" t="s">
+      <c r="C100" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="D100" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="E100" s="9" t="s">
+      <c r="D100" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="E100" s="8" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A101" s="9" t="b">
+      <c r="F100" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H100" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="I100" s="16" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A101" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="B101" s="9" t="s">
+      <c r="B101" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="C101" s="9" t="s">
+      <c r="C101" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="D101" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="E101" s="9" t="s">
+      <c r="D101" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="E101" s="8" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="B102" s="14" t="s">
+      <c r="F101" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H101" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="I101" s="16" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="B102" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="C102" s="14" t="s">
+      <c r="C102" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="D102" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="E102" s="14" t="s">
+      <c r="D102" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E102" s="13" t="s">
         <v>72</v>
       </c>
       <c r="F102" s="1" t="s">
@@ -4019,129 +4205,148 @@
       <c r="G102" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H102" s="17"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B103" s="9" t="s">
+      <c r="H102" s="16"/>
+      <c r="I102" s="16"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A103" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B103" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="C103" s="9" t="s">
+      <c r="C103" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="D103" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="E103" s="9" t="s">
+      <c r="D103" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="E103" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="H103" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B104" s="9" t="s">
+      <c r="H103" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I103" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A104" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B104" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="C104" s="9" t="s">
+      <c r="C104" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="D104" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="E104" s="9" t="s">
+      <c r="D104" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="E104" s="8" t="s">
         <v>113</v>
       </c>
       <c r="H104" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B105" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="I104" s="18" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A105" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B105" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="C105" s="9" t="s">
+      <c r="C105" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="D105" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="E105" s="9" t="s">
+      <c r="D105" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="E105" s="8" t="s">
         <v>122</v>
       </c>
       <c r="H105" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B106" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="I105" s="18" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A106" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B106" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="C106" s="9" t="s">
+      <c r="C106" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="D106" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="E106" s="9" t="s">
+      <c r="D106" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="E106" s="8" t="s">
         <v>123</v>
       </c>
       <c r="H106" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A107" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B107" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="I106" s="18" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A107" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B107" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="C107" s="9" t="s">
+      <c r="C107" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="D107" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="E107" s="9" t="s">
+      <c r="D107" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="E107" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H107" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A108" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B108" s="9" t="s">
+      <c r="H107" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="I107" s="20" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A108" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B108" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="C108" s="9" t="s">
+      <c r="C108" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="D108" s="9" t="s">
+      <c r="D108" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E108" s="9" t="s">
+      <c r="E108" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H108" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H108" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="I108" s="20" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="b">
         <v>1</v>
       </c>
@@ -4157,8 +4362,20 @@
       <c r="E109" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F109" t="s">
+        <v>168</v>
+      </c>
+      <c r="G109" t="s">
+        <v>168</v>
+      </c>
+      <c r="H109" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="I109" s="17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="b">
         <v>0</v>
       </c>
@@ -4174,11 +4391,14 @@
       <c r="E110" t="s">
         <v>27</v>
       </c>
-      <c r="H110" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H110" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I110" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="b">
         <v>0</v>
       </c>
@@ -4194,11 +4414,14 @@
       <c r="E111" t="s">
         <v>15</v>
       </c>
-      <c r="H111" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H111" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I111" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="b">
         <v>0</v>
       </c>
@@ -4214,11 +4437,14 @@
       <c r="E112" t="s">
         <v>24</v>
       </c>
-      <c r="H112" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H112" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I112" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" t="b">
         <v>0</v>
       </c>
@@ -4234,11 +4460,14 @@
       <c r="E113" t="s">
         <v>21</v>
       </c>
-      <c r="H113" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H113" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I113" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" t="b">
         <v>0</v>
       </c>
@@ -4254,11 +4483,14 @@
       <c r="E114" t="s">
         <v>32</v>
       </c>
-      <c r="H114" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H114" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I114" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" t="b">
         <v>0</v>
       </c>
@@ -4274,31 +4506,32 @@
       <c r="E115" t="s">
         <v>115</v>
       </c>
-      <c r="H115" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A116" t="b">
-        <v>0</v>
-      </c>
-      <c r="B116" t="s">
+      <c r="H115" s="17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B116" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C116" t="s">
-        <v>137</v>
-      </c>
-      <c r="D116" s="2" t="s">
+      <c r="C116" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D116" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E116" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H116" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H116" s="16"/>
+      <c r="I116" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" t="b">
         <v>0</v>
       </c>
@@ -4314,11 +4547,11 @@
       <c r="E117" t="s">
         <v>0</v>
       </c>
-      <c r="H117" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I117" s="17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" t="b">
         <v>1</v>
       </c>
@@ -4334,8 +4567,14 @@
       <c r="E118" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H118" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I118" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="b">
         <v>1</v>
       </c>
@@ -4345,7 +4584,7 @@
       <c r="C119" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D119" s="10" t="s">
+      <c r="D119" s="9" t="s">
         <v>151</v>
       </c>
       <c r="E119" s="1" t="s">
@@ -4357,9 +4596,10 @@
       <c r="G119" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H119" s="17"/>
-    </row>
-    <row r="120" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H119" s="16"/>
+      <c r="I119" s="16"/>
+    </row>
+    <row r="120" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="b">
         <v>1</v>
       </c>
@@ -4369,7 +4609,7 @@
       <c r="C120" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D120" s="10" t="s">
+      <c r="D120" s="9" t="s">
         <v>151</v>
       </c>
       <c r="E120" s="1" t="s">
@@ -4381,9 +4621,10 @@
       <c r="G120" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H120" s="17"/>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H120" s="16"/>
+      <c r="I120" s="16"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" t="b">
         <v>1</v>
       </c>
@@ -4399,8 +4640,14 @@
       <c r="E121" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H121" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I121" s="16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="b">
         <v>1</v>
       </c>
@@ -4410,7 +4657,7 @@
       <c r="C122" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D122" s="10" t="s">
+      <c r="D122" s="9" t="s">
         <v>151</v>
       </c>
       <c r="E122" s="1" t="s">
@@ -4422,9 +4669,10 @@
       <c r="G122" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H122" s="17"/>
-    </row>
-    <row r="123" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H122" s="16"/>
+      <c r="I122" s="16"/>
+    </row>
+    <row r="123" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="b">
         <v>1</v>
       </c>
@@ -4434,7 +4682,7 @@
       <c r="C123" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D123" s="10" t="s">
+      <c r="D123" s="9" t="s">
         <v>151</v>
       </c>
       <c r="E123" s="1" t="s">
@@ -4446,9 +4694,10 @@
       <c r="G123" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H123" s="17"/>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H123" s="16"/>
+      <c r="I123" s="16"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" t="b">
         <v>0</v>
       </c>
@@ -4464,28 +4713,44 @@
       <c r="E124" t="s">
         <v>114</v>
       </c>
-      <c r="H124" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A125" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B125" s="9" t="s">
+      <c r="H124" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I124" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A125" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B125" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="C125" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="D125" s="9" t="s">
+      <c r="C125" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D125" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="E125" s="9" t="s">
+      <c r="E125" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="H125" s="18" t="s">
-        <v>159</v>
+      <c r="I125" s="17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>166</v>
+      </c>
+      <c r="B128" s="19" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B129" s="19" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SSDM-8226 Made the test SearchDataSetTest.testSearchWithSampleWithPropertiesThatContains() pass.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01002E5-4433-BF46-9D88-CA1421EF374B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CAC1E4-4995-8E4E-BE8C-F6E1405CDCA6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1600" yWindow="460" windowWidth="36800" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="170">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -533,6 +533,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>+ (?)</t>
   </si>
 </sst>
 </file>
@@ -627,7 +630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -653,6 +656,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1810,8 +1814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659BE2D9-7405-F646-AD2E-50E30EAAC445}">
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G88" sqref="G88"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G106" sqref="G106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2872,12 +2876,6 @@
       <c r="E46" t="s">
         <v>25</v>
       </c>
-      <c r="H46" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="I46" s="17" t="s">
-        <v>164</v>
-      </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="b">
@@ -2895,12 +2893,6 @@
       <c r="E47" t="s">
         <v>34</v>
       </c>
-      <c r="H47" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="I47" s="17" t="s">
-        <v>164</v>
-      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="b">
@@ -2918,12 +2910,6 @@
       <c r="E48" t="s">
         <v>38</v>
       </c>
-      <c r="H48" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="I48" s="17" t="s">
-        <v>164</v>
-      </c>
     </row>
     <row r="49" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="b">
@@ -3085,12 +3071,6 @@
       <c r="E55" t="s">
         <v>17</v>
       </c>
-      <c r="H55" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="I55" s="17" t="s">
-        <v>164</v>
-      </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="b">
@@ -3108,12 +3088,6 @@
       <c r="E56" t="s">
         <v>20</v>
       </c>
-      <c r="H56" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="I56" s="17" t="s">
-        <v>164</v>
-      </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="b">
@@ -3131,12 +3105,6 @@
       <c r="E57" t="s">
         <v>2</v>
       </c>
-      <c r="H57" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="I57" s="17" t="s">
-        <v>164</v>
-      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="b">
@@ -3154,11 +3122,8 @@
       <c r="E58" t="s">
         <v>45</v>
       </c>
-      <c r="H58" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="I58" s="17" t="s">
-        <v>164</v>
+      <c r="I58" s="21" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
@@ -3177,11 +3142,8 @@
       <c r="E59" t="s">
         <v>43</v>
       </c>
-      <c r="H59" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="I59" s="17" t="s">
-        <v>164</v>
+      <c r="I59" s="21" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
@@ -3200,11 +3162,8 @@
       <c r="E60" t="s">
         <v>44</v>
       </c>
-      <c r="H60" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="I60" s="17" t="s">
-        <v>164</v>
+      <c r="I60" s="21" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
@@ -3223,11 +3182,8 @@
       <c r="E61" t="s">
         <v>109</v>
       </c>
-      <c r="H61" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="I61" s="17" t="s">
-        <v>164</v>
+      <c r="I61" s="21" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4224,11 +4180,8 @@
       <c r="E103" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="H103" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="I103" s="17" t="s">
-        <v>164</v>
+      <c r="H103" s="8" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
@@ -4247,12 +4200,10 @@
       <c r="E104" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="H104" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="I104" s="18" t="s">
-        <v>164</v>
-      </c>
+      <c r="H104" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="I104" s="16"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" s="8" t="b">
@@ -4714,10 +4665,7 @@
         <v>114</v>
       </c>
       <c r="H124" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="I124" s="17" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
SSDM-8226 Made the test SearchMaterialTest.testSearchWithTypeWithIdSetToPermId() and SearchLinkDataSetTest.searchWithLegacyExternalDms() pass.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CAC1E4-4995-8E4E-BE8C-F6E1405CDCA6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6017FDA2-1CE8-F74C-9F42-32257469186D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1600" yWindow="460" windowWidth="36800" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="170">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -1814,8 +1814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659BE2D9-7405-F646-AD2E-50E30EAAC445}">
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G106" sqref="G106"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1903,25 +1903,30 @@
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="H4" s="17" t="s">
-        <v>159</v>
-      </c>
+      <c r="F4" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="b">
@@ -2002,25 +2007,30 @@
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="b">
-        <v>0</v>
-      </c>
-      <c r="B8" s="2" t="s">
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H8" s="17" t="s">
-        <v>159</v>
-      </c>
+      <c r="F8" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
     </row>
     <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="b">
@@ -2047,23 +2057,24 @@
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="b">
-        <v>0</v>
-      </c>
-      <c r="B10" s="2" t="s">
+    <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="H10" s="16"/>
+      <c r="I10" s="16" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2464,6 +2475,18 @@
       </c>
       <c r="E27" t="s">
         <v>4</v>
+      </c>
+      <c r="F27" t="s">
+        <v>168</v>
+      </c>
+      <c r="G27" t="s">
+        <v>168</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
SSDM-8226 Plugged new engine for SampleTypeSearchCriteria.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criteria.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6017FDA2-1CE8-F74C-9F42-32257469186D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1987DBFD-1278-444A-B2C2-72E6C4EE2A16}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="460" windowWidth="36800" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
+    <workbookView xWindow="1340" yWindow="460" windowWidth="27460" windowHeight="17540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="176">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -536,6 +537,24 @@
   </si>
   <si>
     <t>+ (?)</t>
+  </si>
+  <si>
+    <t>Tests using SQL translator</t>
+  </si>
+  <si>
+    <t>SearchDataSetTest</t>
+  </si>
+  <si>
+    <t>SearchExperimentTest</t>
+  </si>
+  <si>
+    <t>SearchLinkDataSetTest</t>
+  </si>
+  <si>
+    <t>SearchMaterialTest</t>
+  </si>
+  <si>
+    <t>SearchSampleTest</t>
   </si>
 </sst>
 </file>
@@ -973,7 +992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BFF7087-EBB5-6245-A677-DC1F53C20582}">
   <dimension ref="A1:E128"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
@@ -1811,11 +1830,59 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11ED2671-8FDC-244A-8E4C-353754294D0E}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659BE2D9-7405-F646-AD2E-50E30EAAC445}">
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView topLeftCell="A75" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1903,59 +1970,50 @@
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
     </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B4" s="15" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>130</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>148</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>118</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="b">
+      <c r="H4" s="17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F5" t="s">
-        <v>168</v>
-      </c>
-      <c r="G5" t="s">
-        <v>168</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>168</v>
-      </c>
+      <c r="F5" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="b">
@@ -2007,30 +2065,25 @@
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B8" s="15" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>130</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>141</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>117</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
+      <c r="H8" s="17" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="b">
@@ -2057,24 +2110,23 @@
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
     </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B10" s="15" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="b">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>130</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>149</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>48</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16" t="s">
+      <c r="I10" s="17" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2475,18 +2527,6 @@
       </c>
       <c r="E27" t="s">
         <v>4</v>
-      </c>
-      <c r="F27" t="s">
-        <v>168</v>
-      </c>
-      <c r="G27" t="s">
-        <v>168</v>
-      </c>
-      <c r="H27" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="I27" s="16" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>